<commit_message>
Edit code format and comments
</commit_message>
<xml_diff>
--- a/hemlock_adelgid/ha_data.xlsx
+++ b/hemlock_adelgid/ha_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hannah/Documents/adelgid_models/hemlock_adelgid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86A2BAA-DD20-6544-A96B-FCF312EA5E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2341D53B-EF94-D24B-981D-8D666C4AAF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="25260" windowHeight="15500" activeTab="6" xr2:uid="{059E70AB-59D7-F942-9513-6BE22997322C}"/>
+    <workbookView minimized="1" xWindow="6140" yWindow="500" windowWidth="25260" windowHeight="15500" activeTab="4" xr2:uid="{059E70AB-59D7-F942-9513-6BE22997322C}"/>
   </bookViews>
   <sheets>
     <sheet name="group_1_H" sheetId="1" r:id="rId1"/>
@@ -6067,7 +6067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EFF2204-1BD6-6544-833B-ECA193E80749}">
   <dimension ref="A1:CO18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -9291,7 +9291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD29C8B-ABF3-DE49-9B4F-F275B68EF587}">
   <dimension ref="A1:OI16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>